<commit_message>
Updated group discussion topics
</commit_message>
<xml_diff>
--- a/assets/Students.xlsx
+++ b/assets/Students.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fsm788/Documents/Teaching/Advanced-WIM/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735F7A34-8700-7241-8866-FBC8F00716F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F1A664-FDF8-3441-8BB4-45F6AA8C8A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{4A6DBC21-0A02-1748-BE6E-5E22D5AAB317}"/>
+    <workbookView xWindow="40" yWindow="500" windowWidth="35560" windowHeight="19480" xr2:uid="{4A6DBC21-0A02-1748-BE6E-5E22D5AAB317}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{55D7D5AC-F1FD-0243-9D03-2C78B416ECF0}" name="2022-08-24T1202_Grades-2500-E22;Advanced_welfare,_Inequality_and_Mobility" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/fsm788/Downloads/2022-08-24T1202_Grades-2500-E22;Advanced_welfare,_Inequality_and_Mobility.csv" decimal="," thousands="." tab="0" comma="1">
+    <textPr sourceFile="/Users/fsm788/Downloads/2022-08-24T1202_Grades-2500-E22;Advanced_welfare,_Inequality_and_Mobility.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="17">
         <textField type="text"/>
         <textField/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="112">
   <si>
     <t>Student</t>
   </si>
@@ -321,13 +321,94 @@
   </si>
   <si>
     <t>email</t>
+  </si>
+  <si>
+    <t>2.2 Jackson</t>
+  </si>
+  <si>
+    <t>2.1 Protsch</t>
+  </si>
+  <si>
+    <t>Allister</t>
+  </si>
+  <si>
+    <t>3.2 Kas</t>
+  </si>
+  <si>
+    <t>3.1 Schaeffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clara </t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>4.2 Rijt</t>
+  </si>
+  <si>
+    <t>4.1 Salganik</t>
+  </si>
+  <si>
+    <t>5.1 Calarco</t>
+  </si>
+  <si>
+    <t>5.2 Ying</t>
+  </si>
+  <si>
+    <t>6.1 Lutter</t>
+  </si>
+  <si>
+    <t>Zenia</t>
+  </si>
+  <si>
+    <t>6.2 Godechot</t>
+  </si>
+  <si>
+    <t>Maddison</t>
+  </si>
+  <si>
+    <t>6.2 Anderson</t>
+  </si>
+  <si>
+    <t>7.1 Völker</t>
+  </si>
+  <si>
+    <t>8.1 Jørgensen</t>
+  </si>
+  <si>
+    <t>8.2 Wiedner</t>
+  </si>
+  <si>
+    <t>9.1 Tapia</t>
+  </si>
+  <si>
+    <t>Paulus</t>
+  </si>
+  <si>
+    <t>9.2 Martin-Caughey</t>
+  </si>
+  <si>
+    <t>Kamille</t>
+  </si>
+  <si>
+    <t>10.1 Harris</t>
+  </si>
+  <si>
+    <t>10.2 Vedres</t>
+  </si>
+  <si>
+    <t>11.1 Brüderl</t>
+  </si>
+  <si>
+    <t>11.2 Abbott</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -339,6 +420,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -364,11 +452,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D62A16-0B93-AC4E-83B7-ABAA1789C773}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -718,6 +807,9 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -726,6 +818,9 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -734,6 +829,9 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
+      <c r="C4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -742,6 +840,9 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="C5" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -750,6 +851,9 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -758,6 +862,9 @@
       <c r="B7" t="s">
         <v>12</v>
       </c>
+      <c r="C7" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -766,6 +873,9 @@
       <c r="B8" t="s">
         <v>14</v>
       </c>
+      <c r="C8" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -774,6 +884,9 @@
       <c r="B9" t="s">
         <v>16</v>
       </c>
+      <c r="C9" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -790,6 +903,9 @@
       <c r="B11" t="s">
         <v>20</v>
       </c>
+      <c r="C11" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -798,6 +914,9 @@
       <c r="B12" t="s">
         <v>22</v>
       </c>
+      <c r="C12" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -806,6 +925,9 @@
       <c r="B13" t="s">
         <v>24</v>
       </c>
+      <c r="C13" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -822,6 +944,9 @@
       <c r="B15" t="s">
         <v>28</v>
       </c>
+      <c r="C15" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -830,64 +955,88 @@
       <c r="B16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B19" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B21" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B22" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B23" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -895,148 +1044,255 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B25" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B26" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B27" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B28" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B29" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B30" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B31" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B32" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B33" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B34" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B35" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B36" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B37" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B38" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B39" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B40" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B41" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B42" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Social Capital 2 done
</commit_message>
<xml_diff>
--- a/assets/Students.xlsx
+++ b/assets/Students.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fsm788/Documents/Teaching/Advanced-WIM/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F1A664-FDF8-3441-8BB4-45F6AA8C8A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8D260F-B6B4-1A4A-9783-EFE43179DE1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="500" windowWidth="35560" windowHeight="19480" xr2:uid="{4A6DBC21-0A02-1748-BE6E-5E22D5AAB317}"/>
+    <workbookView xWindow="4800" yWindow="500" windowWidth="28800" windowHeight="19460" xr2:uid="{4A6DBC21-0A02-1748-BE6E-5E22D5AAB317}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="113">
   <si>
     <t>Student</t>
   </si>
@@ -368,9 +368,6 @@
     <t>Maddison</t>
   </si>
   <si>
-    <t>6.2 Anderson</t>
-  </si>
-  <si>
     <t>7.1 Völker</t>
   </si>
   <si>
@@ -402,6 +399,12 @@
   </si>
   <si>
     <t>11.2 Abbott</t>
+  </si>
+  <si>
+    <t>7.2 Anderson</t>
+  </si>
+  <si>
+    <t>Zoe</t>
   </si>
 </sst>
 </file>
@@ -776,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D62A16-0B93-AC4E-83B7-ABAA1789C773}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -802,246 +805,246 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" t="s">
-        <v>106</v>
+        <v>90</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1057,109 +1060,103 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" t="s">
-        <v>94</v>
+        <v>99</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="C35" t="s">
         <v>111</v>
@@ -1167,10 +1164,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s">
         <v>101</v>
@@ -1178,21 +1175,21 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C38" t="s">
         <v>101</v>
@@ -1200,102 +1197,122 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="B41" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>63</v>
+      </c>
+      <c r="C42" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C43" t="s">
-        <v>88</v>
+        <v>104</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
+      </c>
+      <c r="B44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" t="s">
-        <v>92</v>
+        <v>106</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>97</v>
+        <v>17</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
       </c>
       <c r="C46" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>95</v>
+        <v>25</v>
+      </c>
+      <c r="B47" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>104</v>
+        <v>42</v>
+      </c>
+      <c r="B48" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>106</v>
+        <v>77</v>
+      </c>
+      <c r="B49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C50" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C50">
+    <sortCondition ref="C2:C50"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Drafted Sessions 8 and 9
</commit_message>
<xml_diff>
--- a/assets/Students.xlsx
+++ b/assets/Students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fsm788/Documents/Teaching/Advanced-WIM/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8D260F-B6B4-1A4A-9783-EFE43179DE1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF30AAE-3260-CA41-BD76-CF9F81C21E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="500" windowWidth="28800" windowHeight="19460" xr2:uid="{4A6DBC21-0A02-1748-BE6E-5E22D5AAB317}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="114">
   <si>
     <t>Student</t>
   </si>
@@ -405,6 +405,9 @@
   </si>
   <si>
     <t>Zoe</t>
+  </si>
+  <si>
+    <t>Sick</t>
   </si>
 </sst>
 </file>
@@ -781,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D62A16-0B93-AC4E-83B7-ABAA1789C773}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1300,13 +1303,16 @@
       <c r="B49" t="s">
         <v>78</v>
       </c>
+      <c r="C49" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C50" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Little change to about.
</commit_message>
<xml_diff>
--- a/assets/Students.xlsx
+++ b/assets/Students.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fsm788/Documents/Teaching/Advanced-WIM/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF30AAE-3260-CA41-BD76-CF9F81C21E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40A30E6-F5C3-6D42-AE55-396276CAD1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="500" windowWidth="28800" windowHeight="19460" xr2:uid="{4A6DBC21-0A02-1748-BE6E-5E22D5AAB317}"/>
   </bookViews>
@@ -368,9 +368,6 @@
     <t>Maddison</t>
   </si>
   <si>
-    <t>7.1 Völker</t>
-  </si>
-  <si>
     <t>8.1 Jørgensen</t>
   </si>
   <si>
@@ -408,6 +405,9 @@
   </si>
   <si>
     <t>Sick</t>
+  </si>
+  <si>
+    <t>7.1 Stack</t>
   </si>
 </sst>
 </file>
@@ -438,12 +438,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -458,12 +476,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D62A16-0B93-AC4E-83B7-ABAA1789C773}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -814,7 +840,7 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -825,7 +851,7 @@
         <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -836,7 +862,7 @@
         <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -847,7 +873,7 @@
         <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -858,7 +884,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -869,7 +895,7 @@
         <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -880,7 +906,7 @@
         <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -891,7 +917,7 @@
         <v>65</v>
       </c>
       <c r="C9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -902,211 +928,216 @@
         <v>76</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="6" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="6" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="6" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="6" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="6" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="6"/>
+      <c r="C16" s="7" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="6" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C18" t="s">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="6" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="6" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="6" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C22" t="s">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="9" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="9" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="B26" s="9"/>
+      <c r="C26" s="10" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="9" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="9" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="9" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C30" t="s">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1118,7 +1149,7 @@
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1129,7 +1160,7 @@
         <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1140,7 +1171,7 @@
         <v>70</v>
       </c>
       <c r="C33" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1151,7 +1182,7 @@
         <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1162,157 +1193,157 @@
         <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="B42" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="C42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>103</v>
+        <v>62</v>
+      </c>
+      <c r="B43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44" t="s">
-        <v>29</v>
-      </c>
-      <c r="C44" t="s">
-        <v>105</v>
+        <v>103</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>105</v>
+        <v>82</v>
+      </c>
+      <c r="B45" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46" t="s">
-        <v>18</v>
-      </c>
-      <c r="C46" t="s">
-        <v>111</v>
+        <v>105</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B47" t="s">
-        <v>26</v>
+        <v>111</v>
+      </c>
+      <c r="C47" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B50" s="12" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B49" t="s">
-        <v>78</v>
-      </c>
-      <c r="C49" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C50" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>